<commit_message>
changing everything to sync f for better usability
</commit_message>
<xml_diff>
--- a/RingCentralIntern/RingTernStampCard.xlsx
+++ b/RingCentralIntern/RingTernStampCard.xlsx
@@ -407,6 +407,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -438,15 +447,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -800,14 +800,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" ht="16" thickBot="1">
       <c r="A2" s="7"/>
@@ -918,13 +918,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" thickBot="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="19">
         <f xml:space="preserve"> F4 +F5 + F6 + F7</f>
         <v>32.5</v>
@@ -932,14 +932,14 @@
     </row>
     <row r="10" spans="1:6" ht="16" thickBot="1"/>
     <row r="11" spans="1:6">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" ht="16" thickBot="1">
       <c r="A12" s="10"/>
@@ -1061,27 +1061,27 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" thickBot="1">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="19">
         <f xml:space="preserve"> SUM(F13:F17)</f>
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="1:6" ht="16" thickBot="1">
       <c r="A22" s="13"/>
@@ -1202,13 +1202,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" thickBot="1">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="20">
         <f xml:space="preserve"> SUM(F23:F27)</f>
         <v>44</v>
@@ -1216,14 +1216,14 @@
     </row>
     <row r="30" spans="1:6" ht="16" thickBot="1"/>
     <row r="31" spans="1:6">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="32" spans="1:6" ht="16" thickBot="1">
       <c r="A32" s="16"/>
@@ -1250,71 +1250,122 @@
       <c r="B33" s="22">
         <v>0.375</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="6"/>
+      <c r="C33" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="22">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E33" s="22">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F33" s="6">
+        <v>9</v>
+      </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="6"/>
+      <c r="B34" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C34" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="22">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E34" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="F34" s="6">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="6"/>
+      <c r="B35" s="22">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C35" s="22">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D35" s="22">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E35" s="22">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F35" s="6">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="6"/>
+      <c r="B36" s="22">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C36" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="22">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E36" s="22">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F36" s="6">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="16" thickBot="1">
       <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="6"/>
+      <c r="B37" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C37" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="22">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E37" s="22">
+        <v>0.1875</v>
+      </c>
+      <c r="F37" s="6">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="16" thickBot="1">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="20"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="20">
+        <f xml:space="preserve"> SUM(F33:F37)</f>
+        <v>41.5</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="16" thickBot="1"/>
     <row r="41" spans="1:6">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="25"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:6" ht="16" thickBot="1">
       <c r="A42" s="13"/>
@@ -1338,17 +1389,29 @@
       <c r="A43" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="6"/>
+      <c r="B43" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="C43" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="22">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E43" s="22">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F43" s="6">
+        <v>9</v>
+      </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="4"/>
+      <c r="B44" s="22">
+        <v>0.375</v>
+      </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -1385,25 +1448,25 @@
       <c r="F47" s="6"/>
     </row>
     <row r="48" spans="1:6" ht="16" thickBot="1">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
       <c r="F48" s="20"/>
     </row>
     <row r="50" spans="1:6" ht="16" thickBot="1"/>
     <row r="51" spans="1:6">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="25"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="28"/>
     </row>
     <row r="52" spans="1:6" ht="16" thickBot="1">
       <c r="A52" s="16"/>
@@ -1474,25 +1537,25 @@
       <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" ht="16" thickBot="1">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
       <c r="F58" s="20"/>
     </row>
     <row r="60" spans="1:6" ht="16" thickBot="1"/>
     <row r="61" spans="1:6">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="25"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="28"/>
     </row>
     <row r="62" spans="1:6" ht="16" thickBot="1">
       <c r="A62" s="16"/>
@@ -1563,25 +1626,25 @@
       <c r="F67" s="6"/>
     </row>
     <row r="68" spans="1:6" ht="16" thickBot="1">
-      <c r="A68" s="34" t="s">
+      <c r="A68" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="35"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
       <c r="F68" s="20"/>
     </row>
     <row r="70" spans="1:6" ht="16" thickBot="1"/>
     <row r="71" spans="1:6">
-      <c r="A71" s="23" t="s">
+      <c r="A71" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="25"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="27"/>
+      <c r="F71" s="28"/>
     </row>
     <row r="72" spans="1:6" ht="16" thickBot="1">
       <c r="A72" s="13"/>
@@ -1652,25 +1715,25 @@
       <c r="F77" s="6"/>
     </row>
     <row r="78" spans="1:6" ht="16" thickBot="1">
-      <c r="A78" s="34" t="s">
+      <c r="A78" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="36"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="25"/>
       <c r="F78" s="20"/>
     </row>
     <row r="80" spans="1:6" ht="16" thickBot="1"/>
     <row r="81" spans="1:6">
-      <c r="A81" s="23" t="s">
+      <c r="A81" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="25"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="28"/>
     </row>
     <row r="82" spans="1:6" ht="16" thickBot="1">
       <c r="A82" s="13"/>
@@ -1741,25 +1804,25 @@
       <c r="F87" s="6"/>
     </row>
     <row r="88" spans="1:6" ht="16" thickBot="1">
-      <c r="A88" s="34" t="s">
+      <c r="A88" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B88" s="35"/>
-      <c r="C88" s="35"/>
-      <c r="D88" s="35"/>
-      <c r="E88" s="36"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="25"/>
       <c r="F88" s="20"/>
     </row>
     <row r="90" spans="1:6" ht="16" thickBot="1"/>
     <row r="91" spans="1:6">
-      <c r="A91" s="23" t="s">
+      <c r="A91" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="25"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="28"/>
     </row>
     <row r="92" spans="1:6" ht="16" thickBot="1">
       <c r="A92" s="13"/>
@@ -1830,25 +1893,25 @@
       <c r="F97" s="6"/>
     </row>
     <row r="98" spans="1:6" ht="16" thickBot="1">
-      <c r="A98" s="34" t="s">
+      <c r="A98" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B98" s="35"/>
-      <c r="C98" s="35"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="36"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="25"/>
       <c r="F98" s="20"/>
     </row>
     <row r="100" spans="1:6" ht="16" thickBot="1"/>
     <row r="101" spans="1:6">
-      <c r="A101" s="23" t="s">
+      <c r="A101" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B101" s="24"/>
-      <c r="C101" s="24"/>
-      <c r="D101" s="24"/>
-      <c r="E101" s="24"/>
-      <c r="F101" s="25"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="28"/>
     </row>
     <row r="102" spans="1:6" ht="16" thickBot="1">
       <c r="A102" s="13"/>
@@ -1919,25 +1982,25 @@
       <c r="F107" s="6"/>
     </row>
     <row r="108" spans="1:6" ht="16" thickBot="1">
-      <c r="A108" s="34" t="s">
+      <c r="A108" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B108" s="35"/>
-      <c r="C108" s="35"/>
-      <c r="D108" s="35"/>
-      <c r="E108" s="36"/>
+      <c r="B108" s="24"/>
+      <c r="C108" s="24"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="25"/>
       <c r="F108" s="20"/>
     </row>
     <row r="110" spans="1:6" ht="16" thickBot="1"/>
     <row r="111" spans="1:6">
-      <c r="A111" s="23" t="s">
+      <c r="A111" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B111" s="24"/>
-      <c r="C111" s="24"/>
-      <c r="D111" s="24"/>
-      <c r="E111" s="24"/>
-      <c r="F111" s="25"/>
+      <c r="B111" s="27"/>
+      <c r="C111" s="27"/>
+      <c r="D111" s="27"/>
+      <c r="E111" s="27"/>
+      <c r="F111" s="28"/>
     </row>
     <row r="112" spans="1:6" ht="16" thickBot="1">
       <c r="A112" s="13"/>
@@ -2008,17 +2071,28 @@
       <c r="F117" s="6"/>
     </row>
     <row r="118" spans="1:6" ht="16" thickBot="1">
-      <c r="A118" s="34" t="s">
+      <c r="A118" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B118" s="35"/>
-      <c r="C118" s="35"/>
-      <c r="D118" s="35"/>
-      <c r="E118" s="36"/>
+      <c r="B118" s="24"/>
+      <c r="C118" s="24"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="25"/>
       <c r="F118" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A48:E48"/>
     <mergeCell ref="A118:E118"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A61:F61"/>
@@ -2032,17 +2106,6 @@
     <mergeCell ref="A101:F101"/>
     <mergeCell ref="A108:E108"/>
     <mergeCell ref="A111:F111"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A48:E48"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
updated time sheet again
</commit_message>
<xml_diff>
--- a/RingCentralIntern/RingTernStampCard.xlsx
+++ b/RingCentralIntern/RingTernStampCard.xlsx
@@ -413,6 +413,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -444,15 +453,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -812,14 +812,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" ht="16" thickBot="1">
       <c r="A2" s="7"/>
@@ -930,13 +930,13 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" thickBot="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="19">
         <f xml:space="preserve"> F4 +F5 + F6 + F7</f>
         <v>32.5</v>
@@ -944,14 +944,14 @@
     </row>
     <row r="10" spans="1:6" ht="16" thickBot="1"/>
     <row r="11" spans="1:6">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" ht="16" thickBot="1">
       <c r="A12" s="10"/>
@@ -1073,27 +1073,27 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" thickBot="1">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
       <c r="F18" s="19">
         <f xml:space="preserve"> SUM(F13:F17)</f>
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="1:6" ht="16" thickBot="1">
       <c r="A22" s="13"/>
@@ -1214,13 +1214,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="16" thickBot="1">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="20">
         <f xml:space="preserve"> SUM(F23:F27)</f>
         <v>44</v>
@@ -1228,14 +1228,14 @@
     </row>
     <row r="30" spans="1:6" ht="16" thickBot="1"/>
     <row r="31" spans="1:6">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="32" spans="1:6" ht="16" thickBot="1">
       <c r="A32" s="16"/>
@@ -1356,13 +1356,13 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="16" thickBot="1">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="20">
         <f xml:space="preserve"> SUM(F33:F37)</f>
         <v>42.5</v>
@@ -1370,14 +1370,14 @@
     </row>
     <row r="40" spans="1:6" ht="16" thickBot="1"/>
     <row r="41" spans="1:6">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="25"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:6" ht="16" thickBot="1">
       <c r="A42" s="13"/>
@@ -1498,13 +1498,13 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="16" thickBot="1">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
       <c r="F48" s="20">
         <f xml:space="preserve"> SUM(F43:F47)</f>
         <v>43.5</v>
@@ -1512,14 +1512,14 @@
     </row>
     <row r="50" spans="1:6" ht="16" thickBot="1"/>
     <row r="51" spans="1:6">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="25"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="28"/>
     </row>
     <row r="52" spans="1:6" ht="16" thickBot="1">
       <c r="A52" s="16"/>
@@ -1630,13 +1630,13 @@
       <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" ht="16" thickBot="1">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
       <c r="F58" s="20">
         <f xml:space="preserve"> SUM(F53:F57)</f>
         <v>32.5</v>
@@ -1644,14 +1644,14 @@
     </row>
     <row r="60" spans="1:6" ht="16" thickBot="1"/>
     <row r="61" spans="1:6">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="25"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="28"/>
     </row>
     <row r="62" spans="1:6" ht="16" thickBot="1">
       <c r="A62" s="16"/>
@@ -1705,10 +1705,10 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E64" s="22">
-        <v>0.29166666666666669</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="F64" s="6">
-        <v>9.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1742,28 +1742,28 @@
       <c r="F67" s="6"/>
     </row>
     <row r="68" spans="1:6" ht="16" thickBot="1">
-      <c r="A68" s="34" t="s">
+      <c r="A68" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="35"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
       <c r="F68" s="20">
         <f xml:space="preserve"> SUM(F63:F67)</f>
-        <v>19</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16" thickBot="1"/>
     <row r="71" spans="1:6">
-      <c r="A71" s="23" t="s">
+      <c r="A71" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="25"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="27"/>
+      <c r="F71" s="28"/>
     </row>
     <row r="72" spans="1:6" ht="16" thickBot="1">
       <c r="A72" s="13"/>
@@ -1834,25 +1834,25 @@
       <c r="F77" s="6"/>
     </row>
     <row r="78" spans="1:6" ht="16" thickBot="1">
-      <c r="A78" s="34" t="s">
+      <c r="A78" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="36"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="25"/>
       <c r="F78" s="20"/>
     </row>
     <row r="80" spans="1:6" ht="16" thickBot="1"/>
     <row r="81" spans="1:6">
-      <c r="A81" s="23" t="s">
+      <c r="A81" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="25"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="28"/>
     </row>
     <row r="82" spans="1:6" ht="16" thickBot="1">
       <c r="A82" s="13"/>
@@ -1923,25 +1923,25 @@
       <c r="F87" s="6"/>
     </row>
     <row r="88" spans="1:6" ht="16" thickBot="1">
-      <c r="A88" s="34" t="s">
+      <c r="A88" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B88" s="35"/>
-      <c r="C88" s="35"/>
-      <c r="D88" s="35"/>
-      <c r="E88" s="36"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="25"/>
       <c r="F88" s="20"/>
     </row>
     <row r="90" spans="1:6" ht="16" thickBot="1"/>
     <row r="91" spans="1:6">
-      <c r="A91" s="23" t="s">
+      <c r="A91" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="25"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="28"/>
     </row>
     <row r="92" spans="1:6" ht="16" thickBot="1">
       <c r="A92" s="13"/>
@@ -2012,25 +2012,25 @@
       <c r="F97" s="6"/>
     </row>
     <row r="98" spans="1:6" ht="16" thickBot="1">
-      <c r="A98" s="34" t="s">
+      <c r="A98" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B98" s="35"/>
-      <c r="C98" s="35"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="36"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="25"/>
       <c r="F98" s="20"/>
     </row>
     <row r="100" spans="1:6" ht="16" thickBot="1"/>
     <row r="101" spans="1:6">
-      <c r="A101" s="23" t="s">
+      <c r="A101" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B101" s="24"/>
-      <c r="C101" s="24"/>
-      <c r="D101" s="24"/>
-      <c r="E101" s="24"/>
-      <c r="F101" s="25"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="28"/>
     </row>
     <row r="102" spans="1:6" ht="16" thickBot="1">
       <c r="A102" s="13"/>
@@ -2101,25 +2101,25 @@
       <c r="F107" s="6"/>
     </row>
     <row r="108" spans="1:6" ht="16" thickBot="1">
-      <c r="A108" s="34" t="s">
+      <c r="A108" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B108" s="35"/>
-      <c r="C108" s="35"/>
-      <c r="D108" s="35"/>
-      <c r="E108" s="36"/>
+      <c r="B108" s="24"/>
+      <c r="C108" s="24"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="25"/>
       <c r="F108" s="20"/>
     </row>
     <row r="110" spans="1:6" ht="16" thickBot="1"/>
     <row r="111" spans="1:6">
-      <c r="A111" s="23" t="s">
+      <c r="A111" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B111" s="24"/>
-      <c r="C111" s="24"/>
-      <c r="D111" s="24"/>
-      <c r="E111" s="24"/>
-      <c r="F111" s="25"/>
+      <c r="B111" s="27"/>
+      <c r="C111" s="27"/>
+      <c r="D111" s="27"/>
+      <c r="E111" s="27"/>
+      <c r="F111" s="28"/>
     </row>
     <row r="112" spans="1:6" ht="16" thickBot="1">
       <c r="A112" s="13"/>
@@ -2190,17 +2190,28 @@
       <c r="F117" s="6"/>
     </row>
     <row r="118" spans="1:6" ht="16" thickBot="1">
-      <c r="A118" s="34" t="s">
+      <c r="A118" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B118" s="35"/>
-      <c r="C118" s="35"/>
-      <c r="D118" s="35"/>
-      <c r="E118" s="36"/>
+      <c r="B118" s="24"/>
+      <c r="C118" s="24"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="25"/>
       <c r="F118" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A48:E48"/>
     <mergeCell ref="A118:E118"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A61:F61"/>
@@ -2214,17 +2225,6 @@
     <mergeCell ref="A101:F101"/>
     <mergeCell ref="A108:E108"/>
     <mergeCell ref="A111:F111"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A48:E48"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>